<commit_message>
Updated malware Analysis file
</commit_message>
<xml_diff>
--- a/testing/malware analysis.xlsx
+++ b/testing/malware analysis.xlsx
@@ -5,15 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twinklegupta/Documents/UCLA/Spring 17/CS 230/juxtapp project/CS230-Project/testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amehrotra/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1240" windowWidth="28800" windowHeight="14660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$80</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>Malware Benews</t>
   </si>
@@ -95,9 +98,6 @@
     <t>ch.urbantraining.sportcitytour-3.apk</t>
   </si>
   <si>
-    <t>ch.asimove.swisssolidarity-400.apk</t>
-  </si>
-  <si>
     <t>com.parental.control.v4.apk</t>
   </si>
   <si>
@@ -132,6 +132,240 @@
   </si>
   <si>
     <t>net.tecnotopia.SimpleCalculator.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional </t>
+  </si>
+  <si>
+    <t>asimove.swisssolidarity-400.</t>
+  </si>
+  <si>
+    <t>air.beatsgames.bubblespop-1000004</t>
+  </si>
+  <si>
+    <t>air.AutumnFashion-1000003</t>
+  </si>
+  <si>
+    <t>air.black.game.Trucka.Racing-1</t>
+  </si>
+  <si>
+    <t>air.BoyamaOyunu-1000000</t>
+  </si>
+  <si>
+    <t>air.burgerdecoration-1000000</t>
+  </si>
+  <si>
+    <t>air.ClownKiss-1000000</t>
+  </si>
+  <si>
+    <t>air.com.aardman.musicinc-1001000</t>
+  </si>
+  <si>
+    <t>com.a9232458155006478652fb30a.a51984879a-5</t>
+  </si>
+  <si>
+    <t>com.a79826354351e8af4a6de859a.a07757265a-1</t>
+  </si>
+  <si>
+    <t>com.a6485379785011deac77e038a.a52824612a-1</t>
+  </si>
+  <si>
+    <t>com.a4021326435238c01d256ce2a.a17528134a-1</t>
+  </si>
+  <si>
+    <t>com.a3dstudio.memory_game_3D_2012_demo-5</t>
+  </si>
+  <si>
+    <t>com.a387504803528485473c5716a.a75213173a-1</t>
+  </si>
+  <si>
+    <t>com.a29897822153321824194074a.a47679784a-1</t>
+  </si>
+  <si>
+    <t>com.a27015956501431c8d88926a.a38565801a-2</t>
+  </si>
+  <si>
+    <t>com.a214762125540490b35f6624a.a68875047a-2</t>
+  </si>
+  <si>
+    <t>com.a212580322853c6bfd2dd64b6a.a23974995a-2</t>
+  </si>
+  <si>
+    <t>com.a201832112250629afc4df3e2a.a89421792a-2</t>
+  </si>
+  <si>
+    <t>com.a17740059945057a438714777a.a89469600a-1</t>
+  </si>
+  <si>
+    <t>com.a1674527915040882adb4a87a.a12259281a-1</t>
+  </si>
+  <si>
+    <t>com.a1672371917502fd3285858d9a.a14990635a-5</t>
+  </si>
+  <si>
+    <t>com.a1616440966501bc60f2bcc21a.a07497505a-2</t>
+  </si>
+  <si>
+    <t>com.a159513369151f3f1c3752796a.a47649723a-2</t>
+  </si>
+  <si>
+    <t>com.a159064199750ae0fc10a0231a.a68801334a-1</t>
+  </si>
+  <si>
+    <t>com.a15388667985161e2bf574bc3a.a14990399a-2</t>
+  </si>
+  <si>
+    <t>air.com.aardman.musicinc-1002006</t>
+  </si>
+  <si>
+    <t>air.com.ahmettalut.PrincessBarbiMorningRitual-1000000</t>
+  </si>
+  <si>
+    <t>air.com.absolutist.TapBubble-1001006</t>
+  </si>
+  <si>
+    <t>air.com.ao.PonySweetDayCare-1000000</t>
+  </si>
+  <si>
+    <t>air.com.bravostech.dodge-1000001</t>
+  </si>
+  <si>
+    <t>air.polkafashiondressup-1000001</t>
+  </si>
+  <si>
+    <t>air.StickAdultery-1000003</t>
+  </si>
+  <si>
+    <t>air.TeddyHouseEscape-1000000</t>
+  </si>
+  <si>
+    <t>air.Time_To_Escape-1004000</t>
+  </si>
+  <si>
+    <t>chcomm.chcomm-1</t>
+  </si>
+  <si>
+    <t>chris.russell.sixsixsix-23</t>
+  </si>
+  <si>
+    <t>chesspresso.client.android.f-124</t>
+  </si>
+  <si>
+    <t>ciel.app.hellobus-48</t>
+  </si>
+  <si>
+    <t>cityguide.Hildesheim-20</t>
+  </si>
+  <si>
+    <t>cityguide.Marktheidenfeld-20</t>
+  </si>
+  <si>
+    <t>cityguide.Stolberg-6</t>
+  </si>
+  <si>
+    <t>cityguide.Stolberg-2</t>
+  </si>
+  <si>
+    <t>clicapack.com.clicapackapp.coach_driving-1</t>
+  </si>
+  <si>
+    <t>cmb.dipiter.jewelrober-1</t>
+  </si>
+  <si>
+    <t>cn.apps123.shell.zhaoshangjiamengwang-1</t>
+  </si>
+  <si>
+    <t>cn.com.wali.walisms.theme.countrychant-10</t>
+  </si>
+  <si>
+    <t>cn.com.wali.walisms.theme.lighthouse-10</t>
+  </si>
+  <si>
+    <t>cn.emapp.taobaoclient26-24</t>
+  </si>
+  <si>
+    <t>cn.PuZhenHua.senlin-2</t>
+  </si>
+  <si>
+    <t>cn.wintour.dossm2013.gzhxgj.android-248</t>
+  </si>
+  <si>
+    <t>cn.xrong.mobile.test-15</t>
+  </si>
+  <si>
+    <t>cn.zgningbo-2</t>
+  </si>
+  <si>
+    <t>cn.znteam.gonglve.lijiang-130811</t>
+  </si>
+  <si>
+    <t>cnurf.android.simplified-5</t>
+  </si>
+  <si>
+    <t>co.alotus.remotepresenter.client-2</t>
+  </si>
+  <si>
+    <t>co.andgame.permainanperempuan-4</t>
+  </si>
+  <si>
+    <t>co.basheer.animegirlswallpaper-2</t>
+  </si>
+  <si>
+    <t>co.coprime.cypruslivetv2-1</t>
+  </si>
+  <si>
+    <t>co.il.ezappbulthaup-1</t>
+  </si>
+  <si>
+    <t>co.jp.guerrilla_master-1</t>
+  </si>
+  <si>
+    <t>co.osti.iunipd2-131</t>
+  </si>
+  <si>
+    <t>co.sternet.NDJob-2</t>
+  </si>
+  <si>
+    <t>co.uk.crosbyassociates.morganhemp-5</t>
+  </si>
+  <si>
+    <t>co.wallpaper.en.google.Hug.Nature.Live.Wallpaper-30</t>
+  </si>
+  <si>
+    <t>co.za.ideas4apps.articon-2</t>
+  </si>
+  <si>
+    <t>Fico.za.rainisfallinggames.sheepjump-5</t>
+  </si>
+  <si>
+    <t>cobewell.wolwal.mobile.chapters.office-7</t>
+  </si>
+  <si>
+    <t>coglay.akbdaizukanchugokugo-1</t>
+  </si>
+  <si>
+    <t>colintheshots.homelesshomescreen-1</t>
+  </si>
+  <si>
+    <t>coglay.akbdaizukanchugokugo-2</t>
+  </si>
+  <si>
+    <t>colours.kids-1</t>
+  </si>
+  <si>
+    <t>com.a1267715953500d6162df4376a.a18067257a-1</t>
+  </si>
+  <si>
+    <t>com.a106064014354221c551aeb55a.a39875307a-1</t>
+  </si>
+  <si>
+    <t>com.a1286960127517d9de50ced56a.a46084815a-3</t>
+  </si>
+  <si>
+    <t>com.a13952667370475304276-1399985622</t>
+  </si>
+  <si>
+    <t>com.a1460973773504072fb525953a.a44753669a-1</t>
   </si>
 </sst>
 </file>
@@ -167,8 +401,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,9 +694,10 @@
     <col min="1" max="1" width="54.6640625" customWidth="1"/>
     <col min="2" max="2" width="33.1640625" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="69.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,10 +705,13 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -478,10 +719,13 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -489,10 +733,13 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -500,10 +747,13 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -511,21 +761,27 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -533,10 +789,13 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -544,10 +803,13 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -555,10 +817,13 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -566,10 +831,13 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -577,18 +845,355 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D80"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Malware Analysis - final file
</commit_message>
<xml_diff>
--- a/testing/malware analysis.xlsx
+++ b/testing/malware analysis.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24100" windowHeight="14220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Original Clustering" sheetId="1" r:id="rId1"/>
     <sheet name="clusters 4, k=5, m= 240007" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="clusters = 10, k =5, m= 240007" sheetId="3" r:id="rId3"/>
+    <sheet name="clusters = 20 , k=5, m=240007" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="126">
   <si>
     <t>Malware Benews</t>
   </si>
@@ -368,6 +369,45 @@
   </si>
   <si>
     <t>cbc.androidapp-18.out</t>
+  </si>
+  <si>
+    <t>Malware Parental Control</t>
+  </si>
+  <si>
+    <t>Additional</t>
+  </si>
+  <si>
+    <t>Confusion Matrix</t>
+  </si>
+  <si>
+    <t>Note: 2 apps were not processed</t>
+  </si>
+  <si>
+    <t>Other paramters</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precision </t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Success Rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SucessRate = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SucessRate </t>
   </si>
 </sst>
 </file>
@@ -383,7 +423,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,6 +454,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -427,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -436,18 +482,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="31">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -467,7 +515,247 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -790,8 +1078,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1681,10 +1969,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2515,7 +2803,7 @@
         <v xml:space="preserve">Additional </v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
         <v>83</v>
       </c>
@@ -2524,7 +2812,7 @@
         <v xml:space="preserve">Additional </v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
         <v>84</v>
       </c>
@@ -2533,7 +2821,7 @@
         <v xml:space="preserve">Additional </v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
         <v>85</v>
       </c>
@@ -2542,7 +2830,7 @@
         <v xml:space="preserve">Additional </v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C52" t="s">
         <v>86</v>
       </c>
@@ -2551,36 +2839,189 @@
         <v xml:space="preserve">Additional </v>
       </c>
     </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>10</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>11</v>
+      </c>
+      <c r="D59">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>118</v>
+      </c>
+      <c r="C65" t="s">
+        <v>119</v>
+      </c>
+      <c r="D65" t="s">
+        <v>120</v>
+      </c>
+      <c r="E65" t="s">
+        <v>121</v>
+      </c>
+      <c r="F65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66">
+        <v>10</v>
+      </c>
+      <c r="C66">
+        <v>42</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>0.2</v>
+      </c>
+      <c r="F66">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>113</v>
+      </c>
+      <c r="B67">
+        <v>11</v>
+      </c>
+      <c r="C67">
+        <v>20</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0.35</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68">
+        <v>24</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>61</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" s="7">
+        <v>0.42049999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B31">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Additional">
+    <cfRule type="containsText" dxfId="30" priority="7" operator="containsText" text="Additional">
       <formula>NOT(ISERROR(SEARCH("Additional",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D52">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Additional">
+    <cfRule type="containsText" dxfId="29" priority="6" operator="containsText" text="Additional">
       <formula>NOT(ISERROR(SEARCH("Additional",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F22">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Additional">
+    <cfRule type="containsText" dxfId="28" priority="5" operator="containsText" text="Additional">
       <formula>NOT(ISERROR(SEARCH("Additional",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H3">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Additional">
+    <cfRule type="containsText" dxfId="27" priority="4" operator="containsText" text="Additional">
       <formula>NOT(ISERROR(SEARCH("Additional",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Malware Benews">
-      <formula>NOT(ISERROR(SEARCH("Malware Benews",A1)))</formula>
+  <conditionalFormatting sqref="A1:XFD55 A69:XFD1048576 G56:XFD68">
+    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="Malware Trojan">
+      <formula>NOT(ISERROR(SEARCH("Malware Trojan",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Malware parental">
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Malware parental">
       <formula>NOT(ISERROR(SEARCH("Malware parental",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Malware Trojan">
-      <formula>NOT(ISERROR(SEARCH("Malware Trojan",A1)))</formula>
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Malware Benews">
+      <formula>NOT(ISERROR(SEARCH("Malware Benews",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2590,14 +3031,2126 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView showRuler="0" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" t="str">
+        <f>VLOOKUP(A1,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="str">
+        <f>VLOOKUP(C1,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="str">
+        <f>VLOOKUP(E1,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="str">
+        <f>VLOOKUP(G1,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" t="str">
+        <f>VLOOKUP(E2,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="str">
+        <f>VLOOKUP(G2,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="str">
+        <f>VLOOKUP(C3,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" t="str">
+        <f>VLOOKUP(E3,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="str">
+        <f>VLOOKUP(G3,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="str">
+        <f>VLOOKUP(C4,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="str">
+        <f>VLOOKUP(G4,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="str">
+        <f>VLOOKUP(C5,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="str">
+        <f>VLOOKUP(G5,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="str">
+        <f>VLOOKUP(C6,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="str">
+        <f>VLOOKUP(E6,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" t="str">
+        <f>VLOOKUP(G6,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" t="str">
+        <f>VLOOKUP(C7,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="str">
+        <f>VLOOKUP(E7,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="str">
+        <f>VLOOKUP(G7,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" t="str">
+        <f>VLOOKUP(C8,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="str">
+        <f>VLOOKUP(E8,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="str">
+        <f>VLOOKUP(G8,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="str">
+        <f>VLOOKUP(A9,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" t="str">
+        <f>VLOOKUP(C9,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="str">
+        <f>VLOOKUP(E9,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" t="str">
+        <f>VLOOKUP(G9,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="str">
+        <f>VLOOKUP(A10,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" t="str">
+        <f>VLOOKUP(C10,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="str">
+        <f>VLOOKUP(E10,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" t="str">
+        <f>VLOOKUP(G10,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="str">
+        <f>VLOOKUP(A11,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" t="str">
+        <f>VLOOKUP(C11,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="str">
+        <f>VLOOKUP(E11,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" t="str">
+        <f>VLOOKUP(G11,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="str">
+        <f>VLOOKUP(A12,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="str">
+        <f>VLOOKUP(E12,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" t="str">
+        <f>VLOOKUP(G12,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="str">
+        <f>VLOOKUP(A13,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="str">
+        <f>VLOOKUP(C13,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="str">
+        <f>VLOOKUP(E13,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="str">
+        <f>VLOOKUP(G13,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="str">
+        <f>VLOOKUP(A14,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="str">
+        <f>VLOOKUP(C14,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="str">
+        <f>VLOOKUP(E14,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" t="str">
+        <f>VLOOKUP(G14,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="str">
+        <f>VLOOKUP(A15,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="str">
+        <f>VLOOKUP(C15,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="str">
+        <f>VLOOKUP(E15,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" t="str">
+        <f>VLOOKUP(G15,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="str">
+        <f>VLOOKUP(A16,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="str">
+        <f>VLOOKUP(C16,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="str">
+        <f>VLOOKUP(E16,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" t="str">
+        <f>VLOOKUP(G16,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="str">
+        <f>VLOOKUP(C17,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="str">
+        <f>VLOOKUP(E17,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="G17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" t="str">
+        <f>VLOOKUP(G17,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="str">
+        <f>VLOOKUP(C18,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" t="str">
+        <f>VLOOKUP(E18,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="G18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" t="str">
+        <f>VLOOKUP(G18,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="str">
+        <f>VLOOKUP(A19,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="str">
+        <f>VLOOKUP(E19,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="G19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" t="str">
+        <f>VLOOKUP(G19,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="str">
+        <f>VLOOKUP(A20,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" t="str">
+        <f>VLOOKUP(C20,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" t="str">
+        <f>VLOOKUP(E20,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" t="str">
+        <f>VLOOKUP(G20,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="str">
+        <f>VLOOKUP(A21,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" t="str">
+        <f>VLOOKUP(C21,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" t="str">
+        <f>VLOOKUP(E21,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="G21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" t="str">
+        <f>VLOOKUP(G21,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="str">
+        <f>VLOOKUP(A22,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" t="str">
+        <f>VLOOKUP(C22,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" t="str">
+        <f>VLOOKUP(E22,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="G22" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" t="str">
+        <f>VLOOKUP(G22,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="str">
+        <f>VLOOKUP(A23,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" t="str">
+        <f>VLOOKUP(C23,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" t="str">
+        <f>VLOOKUP(E23,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="G23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" t="str">
+        <f>VLOOKUP(G23,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="str">
+        <f>VLOOKUP(A24,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="str">
+        <f>VLOOKUP(E24,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="G24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" t="str">
+        <f>VLOOKUP(G24,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" t="str">
+        <f>VLOOKUP(C25,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="G25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" t="str">
+        <f>VLOOKUP(G25,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" t="str">
+        <f>VLOOKUP(C26,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="G26" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" t="str">
+        <f>VLOOKUP(G26,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" t="str">
+        <f>VLOOKUP(C27,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" t="str">
+        <f>VLOOKUP(G27,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" t="str">
+        <f>VLOOKUP(C28,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="G28" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" t="str">
+        <f>VLOOKUP(G28,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" t="str">
+        <f>VLOOKUP(G29,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" t="str">
+        <f>VLOOKUP(G30,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31" t="str">
+        <f>VLOOKUP(G31,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" t="str">
+        <f>VLOOKUP(G32,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" t="str">
+        <f>VLOOKUP(G33,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" t="str">
+        <f>VLOOKUP(G34,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" t="str">
+        <f>VLOOKUP(G35,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>70</v>
+      </c>
+      <c r="H36" t="str">
+        <f>VLOOKUP(G36,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H37" t="str">
+        <f>VLOOKUP(G37,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>72</v>
+      </c>
+      <c r="H38" t="str">
+        <f>VLOOKUP(G38,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" t="str">
+        <f>VLOOKUP(G39,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>74</v>
+      </c>
+      <c r="H40" t="str">
+        <f>VLOOKUP(G40,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>75</v>
+      </c>
+      <c r="H41" t="str">
+        <f>VLOOKUP(G41,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>9</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>11</v>
+      </c>
+      <c r="D48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" t="s">
+        <v>120</v>
+      </c>
+      <c r="E54" t="s">
+        <v>121</v>
+      </c>
+      <c r="F54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55">
+        <v>9</v>
+      </c>
+      <c r="C55">
+        <v>32</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>0.22</v>
+      </c>
+      <c r="F55">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56">
+        <v>11</v>
+      </c>
+      <c r="C56">
+        <v>8</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57">
+        <v>46</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>39</v>
+      </c>
+      <c r="E57">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="F57">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="7">
+        <v>0.61680000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B24">
+    <cfRule type="containsText" dxfId="23" priority="16" operator="containsText" text="Additional">
+      <formula>NOT(ISERROR(SEARCH("Additional",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B24">
+    <cfRule type="containsText" dxfId="22" priority="13" operator="containsText" text="Malware Trojan">
+      <formula>NOT(ISERROR(SEARCH("Malware Trojan",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Malware parental">
+      <formula>NOT(ISERROR(SEARCH("Malware parental",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Malware Benews">
+      <formula>NOT(ISERROR(SEARCH("Malware Benews",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D28">
+    <cfRule type="containsText" dxfId="19" priority="12" operator="containsText" text="Additional">
+      <formula>NOT(ISERROR(SEARCH("Additional",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D28">
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Malware Trojan">
+      <formula>NOT(ISERROR(SEARCH("Malware Trojan",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Malware parental">
+      <formula>NOT(ISERROR(SEARCH("Malware parental",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="Malware Benews">
+      <formula>NOT(ISERROR(SEARCH("Malware Benews",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F24">
+    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="Additional">
+      <formula>NOT(ISERROR(SEARCH("Additional",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F24">
+    <cfRule type="containsText" dxfId="14" priority="5" operator="containsText" text="Malware Trojan">
+      <formula>NOT(ISERROR(SEARCH("Malware Trojan",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="Malware parental">
+      <formula>NOT(ISERROR(SEARCH("Malware parental",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="Malware Benews">
+      <formula>NOT(ISERROR(SEARCH("Malware Benews",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H41">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Additional">
+      <formula>NOT(ISERROR(SEARCH("Additional",H1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H41">
+    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Malware Trojan">
+      <formula>NOT(ISERROR(SEARCH("Malware Trojan",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="Malware parental">
+      <formula>NOT(ISERROR(SEARCH("Malware parental",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Malware Benews">
+      <formula>NOT(ISERROR(SEARCH("Malware Benews",H1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F67"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="str">
+        <f>VLOOKUP(A1,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="str">
+        <f>VLOOKUP(C1,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" t="str">
+        <f>VLOOKUP(E1,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" t="str">
+        <f>VLOOKUP(E2,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="str">
+        <f>VLOOKUP(C3,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="str">
+        <f>VLOOKUP(C4,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="str">
+        <f>VLOOKUP(E4,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="str">
+        <f>VLOOKUP(C5,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="str">
+        <f>VLOOKUP(E5,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="str">
+        <f>VLOOKUP(C6,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="str">
+        <f>VLOOKUP(E6,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="str">
+        <f>VLOOKUP(C7,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="str">
+        <f>VLOOKUP(E7,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="str">
+        <f>VLOOKUP(C8,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="str">
+        <f>VLOOKUP(E8,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" t="str">
+        <f>VLOOKUP(A9,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="str">
+        <f>VLOOKUP(C9,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" t="str">
+        <f>VLOOKUP(A10,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="str">
+        <f>VLOOKUP(C10,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="str">
+        <f>VLOOKUP(E10,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="str">
+        <f>VLOOKUP(A11,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="str">
+        <f>VLOOKUP(C11,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="str">
+        <f>VLOOKUP(E11,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="str">
+        <f>VLOOKUP(C12,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="str">
+        <f>VLOOKUP(E12,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="str">
+        <f>VLOOKUP(C13,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="str">
+        <f>VLOOKUP(E13,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" t="str">
+        <f>VLOOKUP(A14,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" t="str">
+        <f>VLOOKUP(C14,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="str">
+        <f>VLOOKUP(E14,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" t="str">
+        <f>VLOOKUP(A15,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="str">
+        <f>VLOOKUP(C15,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" t="str">
+        <f>VLOOKUP(A16,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="str">
+        <f>VLOOKUP(C16,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" t="str">
+        <f>VLOOKUP(C17,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" t="str">
+        <f>VLOOKUP(E17,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="str">
+        <f>VLOOKUP(A18,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="str">
+        <f>VLOOKUP(C18,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" t="str">
+        <f>VLOOKUP(E18,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="str">
+        <f>VLOOKUP(A19,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="str">
+        <f>VLOOKUP(C19,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" t="str">
+        <f>VLOOKUP(E19,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" t="str">
+        <f>VLOOKUP(A20,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" t="str">
+        <f>VLOOKUP(C20,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" t="str">
+        <f>VLOOKUP(E20,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" t="str">
+        <f>VLOOKUP(A21,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" t="str">
+        <f>VLOOKUP(C21,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" t="str">
+        <f>VLOOKUP(E21,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="str">
+        <f>VLOOKUP(C22,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" t="str">
+        <f>VLOOKUP(E22,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="str">
+        <f>VLOOKUP(A23,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="str">
+        <f>VLOOKUP(C23,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" t="str">
+        <f>VLOOKUP(E23,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="str">
+        <f>VLOOKUP(A24,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="str">
+        <f>VLOOKUP(C24,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" t="str">
+        <f>VLOOKUP(E24,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" t="str">
+        <f>VLOOKUP(C25,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" t="str">
+        <f>VLOOKUP(E25,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="str">
+        <f>VLOOKUP(A26,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" t="str">
+        <f>VLOOKUP(C26,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="str">
+        <f>VLOOKUP(A27,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" t="str">
+        <f>VLOOKUP(C27,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" t="str">
+        <f>VLOOKUP(E27,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" t="str">
+        <f>VLOOKUP(A28,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" t="str">
+        <f>VLOOKUP(C28,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E28" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" t="str">
+        <f>VLOOKUP(E28,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="str">
+        <f>VLOOKUP(A29,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" t="str">
+        <f>VLOOKUP(C29,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" t="str">
+        <f>VLOOKUP(A30,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="C30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" t="str">
+        <f>VLOOKUP(C30,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" t="str">
+        <f>VLOOKUP(E30,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="str">
+        <f>VLOOKUP(A31,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="C31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" t="str">
+        <f>VLOOKUP(C31,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+      <c r="E31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" t="str">
+        <f>VLOOKUP(E31,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" t="str">
+        <f>VLOOKUP(A32,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" t="str">
+        <f>VLOOKUP(A33,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" t="str">
+        <f>VLOOKUP(E33,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" t="str">
+        <f>VLOOKUP(A34,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="C34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" t="str">
+        <f>VLOOKUP(C34,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" t="str">
+        <f>VLOOKUP(E34,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" t="str">
+        <f>VLOOKUP(A35,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" t="str">
+        <f>VLOOKUP(C35,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" t="str">
+        <f>VLOOKUP(A36,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware parental control</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="str">
+        <f>VLOOKUP(C37,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="str">
+        <f>VLOOKUP(C38,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="str">
+        <f>VLOOKUP(A39,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" t="str">
+        <f>VLOOKUP(A40,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" t="str">
+        <f>VLOOKUP(A41,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="str">
+        <f>VLOOKUP(C41,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" t="str">
+        <f>VLOOKUP(A42,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="str">
+        <f>VLOOKUP(C42,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" t="str">
+        <f>VLOOKUP(C43,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" t="str">
+        <f>VLOOKUP(A44,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" t="str">
+        <f>VLOOKUP(C44,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" t="str">
+        <f>VLOOKUP(A45,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Trojan</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" t="str">
+        <f>VLOOKUP(C45,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v>Malware Benews</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" t="str">
+        <f>VLOOKUP(C46,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>109</v>
+      </c>
+      <c r="B47" t="str">
+        <f>VLOOKUP(A47,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" t="str">
+        <f>VLOOKUP(A49,'Original Clustering'!$A$1:$B$109,2,FALSE)</f>
+        <v xml:space="preserve">Additional </v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>11</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>114</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" t="s">
+        <v>119</v>
+      </c>
+      <c r="D62" t="s">
+        <v>120</v>
+      </c>
+      <c r="E62" t="s">
+        <v>121</v>
+      </c>
+      <c r="F62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>6</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>0.45450000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>113</v>
+      </c>
+      <c r="B64">
+        <v>11</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65">
+        <v>85</v>
+      </c>
+      <c r="C65">
+        <v>6</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>123</v>
+      </c>
+      <c r="B67" s="7">
+        <v>0.94389999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B49 F1:F40">
+    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="Additional">
+      <formula>NOT(ISERROR(SEARCH("Additional",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B49 F1:F40">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Malware Trojan">
+      <formula>NOT(ISERROR(SEARCH("Malware Trojan",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="Malware parental">
+      <formula>NOT(ISERROR(SEARCH("Malware parental",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="11" operator="containsText" text="Malware Benews">
+      <formula>NOT(ISERROR(SEARCH("Malware Benews",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D46">
+    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="Additional">
+      <formula>NOT(ISERROR(SEARCH("Additional",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D46">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Malware Trojan">
+      <formula>NOT(ISERROR(SEARCH("Malware Trojan",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="Malware parental">
+      <formula>NOT(ISERROR(SEARCH("Malware parental",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="Malware Benews">
+      <formula>NOT(ISERROR(SEARCH("Malware Benews",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>